<commit_message>
Update Log4j2 to version 2.17.1. Ready to assemble Maven
</commit_message>
<xml_diff>
--- a/src/main/resources/template/QR-Code.xlsx
+++ b/src/main/resources/template/QR-Code.xlsx
@@ -349,9 +349,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.11811023622047245" right="0" top="3.937007874015748E-2" bottom="0" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Сustomizing tag qr-code(edited toFormQrCode)
</commit_message>
<xml_diff>
--- a/src/main/resources/template/QR-Code.xlsx
+++ b/src/main/resources/template/QR-Code.xlsx
@@ -347,15 +347,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="214" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.11811023622047245" right="0" top="3.937007874015748E-2" bottom="0" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Updated background anchorPane and optimized qr-code size to 40X30("QR-CODE.xlsx")
</commit_message>
<xml_diff>
--- a/src/main/resources/template/QR-Code.xlsx
+++ b/src/main/resources/template/QR-Code.xlsx
@@ -347,13 +347,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="214" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -367,7 +370,8 @@
     <row r="9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.11811023622047245" right="0" top="3.937007874015748E-2" bottom="0" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <printOptions verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="7.874015748031496E-2" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>